<commit_message>
length compare plots in latex
</commit_message>
<xml_diff>
--- a/Data/t_test_results.xlsx
+++ b/Data/t_test_results.xlsx
@@ -1487,8 +1487,12 @@
       <c r="F30" t="n">
         <v>0.3558668750771353</v>
       </c>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>-1.14473713164009</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.26055311655631</v>
+      </c>
       <c r="I30" t="inlineStr">
         <is>
           <t>No</t>
@@ -1508,7 +1512,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>least_to_most</t>
+          <t>manual_few_shot</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1520,10 +1524,14 @@
         <v>0.3337785584068508</v>
       </c>
       <c r="F31" t="n">
-        <v>0.3498959518962656</v>
-      </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+        <v>0.3487301702745721</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-0.9872890808083997</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.3292918121132551</v>
+      </c>
       <c r="I31" t="inlineStr">
         <is>
           <t>No</t>
@@ -1543,7 +1551,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>manual_cot</t>
+          <t>self_refine</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1555,10 +1563,14 @@
         <v>0.3337785584068508</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3551923713253787</v>
-      </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
+        <v>0.351156728855353</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-1.829021014606149</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.07672940280202731</v>
+      </c>
       <c r="I32" t="inlineStr">
         <is>
           <t>No</t>
@@ -1578,7 +1590,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>manual_few_shot</t>
+          <t>tree_of_thought</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1590,10 +1602,14 @@
         <v>0.3337785584068508</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3487301702745721</v>
-      </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
+        <v>0.3478996421926851</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-1.111119966153743</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.2829354362531543</v>
+      </c>
       <c r="I33" t="inlineStr">
         <is>
           <t>No</t>
@@ -1613,7 +1629,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>self_refine</t>
+          <t>zero_shot_cot</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1625,10 +1641,14 @@
         <v>0.3337785584068508</v>
       </c>
       <c r="F34" t="n">
-        <v>0.351156728855353</v>
-      </c>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
+        <v>0.3441867682123834</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-1.298666300051236</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.2018843348096545</v>
+      </c>
       <c r="I34" t="inlineStr">
         <is>
           <t>No</t>
@@ -1648,7 +1668,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>tree_of_thought</t>
+          <t>least_to_most</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1660,13 +1680,17 @@
         <v>0.3337785584068508</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3478996421926851</v>
-      </c>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+        <v>0.3498959518962656</v>
+      </c>
+      <c r="G35" t="n">
+        <v>-2.408247956271698</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.02196460748337448</v>
+      </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -1683,7 +1707,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>zero_shot_cot</t>
+          <t>manual_cot</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1695,13 +1719,17 @@
         <v>0.3337785584068508</v>
       </c>
       <c r="F36" t="n">
-        <v>0.3441867682123834</v>
-      </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+        <v>0.3551923713253787</v>
+      </c>
+      <c r="G36" t="n">
+        <v>-2.374394674574453</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.02374316969700669</v>
+      </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -1935,7 +1963,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ape_zero_shot_cot</t>
+          <t>least_to_most</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1947,10 +1975,14 @@
         <v>0.367653995409958</v>
       </c>
       <c r="F44" t="n">
-        <v>0.3910591202955087</v>
-      </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
+        <v>0.3688316461987508</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-0.4098421582418101</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.6877150738021158</v>
+      </c>
       <c r="I44" t="inlineStr">
         <is>
           <t>No</t>
@@ -1970,7 +2002,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>least_to_most</t>
+          <t>manual_cot</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1982,10 +2014,14 @@
         <v>0.367653995409958</v>
       </c>
       <c r="F45" t="n">
-        <v>0.3688316461987508</v>
-      </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+        <v>0.3506891984872582</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.2506884562793319</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.8076843000403842</v>
+      </c>
       <c r="I45" t="inlineStr">
         <is>
           <t>No</t>
@@ -2005,7 +2041,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>manual_cot</t>
+          <t>manual_few_shot</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2017,10 +2053,14 @@
         <v>0.367653995409958</v>
       </c>
       <c r="F46" t="n">
-        <v>0.3506891984872582</v>
-      </c>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+        <v>0.363439672985659</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-1.099920436908166</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.2814470372062072</v>
+      </c>
       <c r="I46" t="inlineStr">
         <is>
           <t>No</t>
@@ -2040,7 +2080,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>manual_few_shot</t>
+          <t>self_refine</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2052,10 +2092,14 @@
         <v>0.367653995409958</v>
       </c>
       <c r="F47" t="n">
-        <v>0.363439672985659</v>
-      </c>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
+        <v>0.3927645311833518</v>
+      </c>
+      <c r="G47" t="n">
+        <v>-1.881009639850796</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.07624865825236271</v>
+      </c>
       <c r="I47" t="inlineStr">
         <is>
           <t>No</t>
@@ -2075,7 +2119,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>self_refine</t>
+          <t>tree_of_thought</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2087,10 +2131,14 @@
         <v>0.367653995409958</v>
       </c>
       <c r="F48" t="n">
-        <v>0.3927645311833518</v>
-      </c>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
+        <v>0.3970522049201494</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-0.178304072906799</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.8876686001034875</v>
+      </c>
       <c r="I48" t="inlineStr">
         <is>
           <t>No</t>
@@ -2110,7 +2158,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>tree_of_thought</t>
+          <t>zero_shot_cot</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2122,10 +2170,14 @@
         <v>0.367653995409958</v>
       </c>
       <c r="F49" t="n">
-        <v>0.3970522049201494</v>
-      </c>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
+        <v>0.3859400964114446</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.09440419099120144</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.9255118747930475</v>
+      </c>
       <c r="I49" t="inlineStr">
         <is>
           <t>No</t>
@@ -2145,7 +2197,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>zero_shot_cot</t>
+          <t>ape_zero_shot_cot</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2157,13 +2209,17 @@
         <v>0.367653995409958</v>
       </c>
       <c r="F50" t="n">
-        <v>0.3859400964114446</v>
-      </c>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
+        <v>0.3910591202955087</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-2.106654550723698</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.04734782328834347</v>
+      </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2528,8 +2584,12 @@
       <c r="F61" t="n">
         <v>0.4471702245404097</v>
       </c>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
+      <c r="G61" t="n">
+        <v>0.380597446300002</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.7049950980741344</v>
+      </c>
       <c r="I61" t="inlineStr">
         <is>
           <t>No</t>
@@ -2883,7 +2943,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ape_zero_shot_cot</t>
+          <t>self_refine</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2895,10 +2955,14 @@
         <v>0.3588432399246042</v>
       </c>
       <c r="F72" t="n">
-        <v>0.4195166577919803</v>
-      </c>
-      <c r="G72" t="inlineStr"/>
-      <c r="H72" t="inlineStr"/>
+        <v>0.3655432912693316</v>
+      </c>
+      <c r="G72" t="n">
+        <v>-0.1770794927771922</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.859867225764093</v>
+      </c>
       <c r="I72" t="inlineStr">
         <is>
           <t>No</t>
@@ -2918,7 +2982,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>least_to_most</t>
+          <t>tree_of_thought</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2930,10 +2994,14 @@
         <v>0.3588432399246042</v>
       </c>
       <c r="F73" t="n">
-        <v>0.4795389905014912</v>
-      </c>
-      <c r="G73" t="inlineStr"/>
-      <c r="H73" t="inlineStr"/>
+        <v>0.4301229604135541</v>
+      </c>
+      <c r="G73" t="n">
+        <v>-1.462963211730259</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.1550220395534408</v>
+      </c>
       <c r="I73" t="inlineStr">
         <is>
           <t>No</t>
@@ -2953,7 +3021,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>manual_cot</t>
+          <t>ape_zero_shot_cot</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2965,13 +3033,17 @@
         <v>0.3588432399246042</v>
       </c>
       <c r="F74" t="n">
-        <v>0.4786850615266719</v>
-      </c>
-      <c r="G74" t="inlineStr"/>
-      <c r="H74" t="inlineStr"/>
+        <v>0.4195166577919803</v>
+      </c>
+      <c r="G74" t="n">
+        <v>-2.722508804502758</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.007912598988651227</v>
+      </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -2988,7 +3060,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>manual_few_shot</t>
+          <t>least_to_most</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -3000,13 +3072,17 @@
         <v>0.3588432399246042</v>
       </c>
       <c r="F75" t="n">
-        <v>0.4762447813337619</v>
-      </c>
-      <c r="G75" t="inlineStr"/>
-      <c r="H75" t="inlineStr"/>
+        <v>0.4795389905014912</v>
+      </c>
+      <c r="G75" t="n">
+        <v>-5.704818886801226</v>
+      </c>
+      <c r="H75" t="n">
+        <v>1.37328393154626e-07</v>
+      </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3023,7 +3099,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>self_refine</t>
+          <t>manual_cot</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3035,13 +3111,17 @@
         <v>0.3588432399246042</v>
       </c>
       <c r="F76" t="n">
-        <v>0.3655432912693316</v>
-      </c>
-      <c r="G76" t="inlineStr"/>
-      <c r="H76" t="inlineStr"/>
+        <v>0.4786850615266719</v>
+      </c>
+      <c r="G76" t="n">
+        <v>-5.848788038540913</v>
+      </c>
+      <c r="H76" t="n">
+        <v>7.151516652751101e-08</v>
+      </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3058,7 +3138,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>tree_of_thought</t>
+          <t>manual_few_shot</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3070,13 +3150,17 @@
         <v>0.3588432399246042</v>
       </c>
       <c r="F77" t="n">
-        <v>0.4301229604135541</v>
-      </c>
-      <c r="G77" t="inlineStr"/>
-      <c r="H77" t="inlineStr"/>
+        <v>0.4762447813337619</v>
+      </c>
+      <c r="G77" t="n">
+        <v>-5.402586153841306</v>
+      </c>
+      <c r="H77" t="n">
+        <v>4.852185926605229e-07</v>
+      </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3107,11 +3191,15 @@
       <c r="F78" t="n">
         <v>0.4095443677664702</v>
       </c>
-      <c r="G78" t="inlineStr"/>
-      <c r="H78" t="inlineStr"/>
+      <c r="G78" t="n">
+        <v>-2.345575437840131</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.02150696795521951</v>
+      </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3359,8 +3447,12 @@
       <c r="F86" t="n">
         <v>0.4486177373839107</v>
       </c>
-      <c r="G86" t="inlineStr"/>
-      <c r="H86" t="inlineStr"/>
+      <c r="G86" t="n">
+        <v>-0.5706359002568039</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0.5721119861438464</v>
+      </c>
       <c r="I86" t="inlineStr">
         <is>
           <t>No</t>
@@ -3394,8 +3486,12 @@
       <c r="F87" t="n">
         <v>0.4035677984709117</v>
       </c>
-      <c r="G87" t="inlineStr"/>
-      <c r="H87" t="inlineStr"/>
+      <c r="G87" t="n">
+        <v>-0.04573220039524427</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.9638079071817984</v>
+      </c>
       <c r="I87" t="inlineStr">
         <is>
           <t>No</t>
@@ -3429,8 +3525,12 @@
       <c r="F88" t="n">
         <v>0.4232227201267702</v>
       </c>
-      <c r="G88" t="inlineStr"/>
-      <c r="H88" t="inlineStr"/>
+      <c r="G88" t="n">
+        <v>-0.5956350360123538</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.5556087468580261</v>
+      </c>
       <c r="I88" t="inlineStr">
         <is>
           <t>No</t>
@@ -3450,7 +3550,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>manual_few_shot</t>
+          <t>self_refine</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3462,10 +3562,14 @@
         <v>0.4204354839738638</v>
       </c>
       <c r="F89" t="n">
-        <v>0.3657057845474713</v>
-      </c>
-      <c r="G89" t="inlineStr"/>
-      <c r="H89" t="inlineStr"/>
+        <v>0.3976991678288766</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0.1304041786778109</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0.8970629935145363</v>
+      </c>
       <c r="I89" t="inlineStr">
         <is>
           <t>No</t>
@@ -3485,7 +3589,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>self_refine</t>
+          <t>tree_of_thought</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3497,10 +3601,14 @@
         <v>0.4204354839738638</v>
       </c>
       <c r="F90" t="n">
-        <v>0.3976991678288766</v>
-      </c>
-      <c r="G90" t="inlineStr"/>
-      <c r="H90" t="inlineStr"/>
+        <v>0.4552911088706001</v>
+      </c>
+      <c r="G90" t="n">
+        <v>1.232568738202675</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.2355418166853398</v>
+      </c>
       <c r="I90" t="inlineStr">
         <is>
           <t>No</t>
@@ -3520,7 +3628,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>tree_of_thought</t>
+          <t>manual_few_shot</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3532,13 +3640,17 @@
         <v>0.4204354839738638</v>
       </c>
       <c r="F91" t="n">
-        <v>0.4552911088706001</v>
-      </c>
-      <c r="G91" t="inlineStr"/>
-      <c r="H91" t="inlineStr"/>
+        <v>0.3657057845474713</v>
+      </c>
+      <c r="G91" t="n">
+        <v>2.658636260743372</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.01113814179210349</v>
+      </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3569,11 +3681,15 @@
       <c r="F92" t="n">
         <v>0.4631258808051564</v>
       </c>
-      <c r="G92" t="inlineStr"/>
-      <c r="H92" t="inlineStr"/>
+      <c r="G92" t="n">
+        <v>-2.51052457717059</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.01643009978264356</v>
+      </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -3821,8 +3937,12 @@
       <c r="F100" t="n">
         <v>0.3888047487967222</v>
       </c>
-      <c r="G100" t="inlineStr"/>
-      <c r="H100" t="inlineStr"/>
+      <c r="G100" t="n">
+        <v>-0.5398998232920198</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0.5949457001656505</v>
+      </c>
       <c r="I100" t="inlineStr">
         <is>
           <t>No</t>
@@ -3856,8 +3976,12 @@
       <c r="F101" t="n">
         <v>0.4136875478682511</v>
       </c>
-      <c r="G101" t="inlineStr"/>
-      <c r="H101" t="inlineStr"/>
+      <c r="G101" t="n">
+        <v>-0.09070866577678419</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0.9289243014000621</v>
+      </c>
       <c r="I101" t="inlineStr">
         <is>
           <t>No</t>
@@ -3891,8 +4015,12 @@
       <c r="F102" t="n">
         <v>0.4011686078217538</v>
       </c>
-      <c r="G102" t="inlineStr"/>
-      <c r="H102" t="inlineStr"/>
+      <c r="G102" t="n">
+        <v>-0.68775779570202</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.5089404360165983</v>
+      </c>
       <c r="I102" t="inlineStr">
         <is>
           <t>No</t>
@@ -3912,7 +4040,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>manual_few_shot</t>
+          <t>self_refine</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3924,10 +4052,14 @@
         <v>0.370674139241628</v>
       </c>
       <c r="F103" t="n">
-        <v>0.433228101589585</v>
-      </c>
-      <c r="G103" t="inlineStr"/>
-      <c r="H103" t="inlineStr"/>
+        <v>0.3403139039125427</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0.6324113498329108</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.5350696318477244</v>
+      </c>
       <c r="I103" t="inlineStr">
         <is>
           <t>No</t>
@@ -3947,7 +4079,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>self_refine</t>
+          <t>tree_of_thought</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3959,10 +4091,14 @@
         <v>0.370674139241628</v>
       </c>
       <c r="F104" t="n">
-        <v>0.3403139039125427</v>
-      </c>
-      <c r="G104" t="inlineStr"/>
-      <c r="H104" t="inlineStr"/>
+        <v>0.223879186997216</v>
+      </c>
+      <c r="G104" t="n">
+        <v>1.241549692571777</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0.4316614758653485</v>
+      </c>
       <c r="I104" t="inlineStr">
         <is>
           <t>No</t>
@@ -3982,7 +4118,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>tree_of_thought</t>
+          <t>zero_shot_cot</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3994,10 +4130,14 @@
         <v>0.370674139241628</v>
       </c>
       <c r="F105" t="n">
-        <v>0.223879186997216</v>
-      </c>
-      <c r="G105" t="inlineStr"/>
-      <c r="H105" t="inlineStr"/>
+        <v>0.3573737035024921</v>
+      </c>
+      <c r="G105" t="n">
+        <v>1.439058993114993</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0.1620648744709412</v>
+      </c>
       <c r="I105" t="inlineStr">
         <is>
           <t>No</t>
@@ -4017,7 +4157,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>zero_shot_cot</t>
+          <t>manual_few_shot</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -4029,13 +4169,17 @@
         <v>0.370674139241628</v>
       </c>
       <c r="F106" t="n">
-        <v>0.3573737035024921</v>
-      </c>
-      <c r="G106" t="inlineStr"/>
-      <c r="H106" t="inlineStr"/>
+        <v>0.433228101589585</v>
+      </c>
+      <c r="G106" t="n">
+        <v>-2.928667469841096</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0.006993274462604279</v>
+      </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8427,11 +8571,15 @@
       <c r="F226" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="G226" t="inlineStr"/>
-      <c r="H226" t="inlineStr"/>
+      <c r="G226" t="n">
+        <v>-29.84962311319859</v>
+      </c>
+      <c r="H226" t="n">
+        <v>2.597549811426689e-10</v>
+      </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8462,11 +8610,15 @@
       <c r="F227" t="n">
         <v>7.3</v>
       </c>
-      <c r="G227" t="inlineStr"/>
-      <c r="H227" t="inlineStr"/>
+      <c r="G227" t="n">
+        <v>-26.70571328295164</v>
+      </c>
+      <c r="H227" t="n">
+        <v>7.000859820572747e-10</v>
+      </c>
       <c r="I227" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8497,11 +8649,15 @@
       <c r="F228" t="n">
         <v>3.2</v>
       </c>
-      <c r="G228" t="inlineStr"/>
-      <c r="H228" t="inlineStr"/>
+      <c r="G228" t="n">
+        <v>-2.954195783503986</v>
+      </c>
+      <c r="H228" t="n">
+        <v>0.01611071653191161</v>
+      </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8532,11 +8688,15 @@
       <c r="F229" t="n">
         <v>4.4</v>
       </c>
-      <c r="G229" t="inlineStr"/>
-      <c r="H229" t="inlineStr"/>
+      <c r="G229" t="n">
+        <v>-11.22497216032182</v>
+      </c>
+      <c r="H229" t="n">
+        <v>1.356959540831356e-06</v>
+      </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8567,11 +8727,15 @@
       <c r="F230" t="n">
         <v>4.5</v>
       </c>
-      <c r="G230" t="inlineStr"/>
-      <c r="H230" t="inlineStr"/>
+      <c r="G230" t="n">
+        <v>-9.221981556055331</v>
+      </c>
+      <c r="H230" t="n">
+        <v>6.992072395885232e-06</v>
+      </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8602,11 +8766,15 @@
       <c r="F231" t="n">
         <v>4.2</v>
       </c>
-      <c r="G231" t="inlineStr"/>
-      <c r="H231" t="inlineStr"/>
+      <c r="G231" t="n">
+        <v>-11.75894243853278</v>
+      </c>
+      <c r="H231" t="n">
+        <v>9.151111215642479e-07</v>
+      </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -8637,11 +8805,15 @@
       <c r="F232" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="G232" t="inlineStr"/>
-      <c r="H232" t="inlineStr"/>
+      <c r="G232" t="n">
+        <v>-40.41658075592244</v>
+      </c>
+      <c r="H232" t="n">
+        <v>1.73010492641202e-11</v>
+      </c>
       <c r="I232" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>

</xml_diff>